<commit_message>
Se trabajo en modulo cliente
</commit_message>
<xml_diff>
--- a/Excel/reporte_productos.xlsx
+++ b/Excel/reporte_productos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>Reporte de productos en Excel</t>
   </si>
@@ -47,139 +47,79 @@
     <t>precio</t>
   </si>
   <si>
-    <t xml:space="preserve">Acetaminofen </t>
-  </si>
-  <si>
-    <t>X 150 mg / 5 mL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JARABE </t>
-  </si>
-  <si>
-    <t>Abbott Laboratories</t>
-  </si>
-  <si>
-    <t>Ampolla</t>
-  </si>
-  <si>
-    <t>Cápsula</t>
-  </si>
-  <si>
-    <t>Advil Gripa</t>
-  </si>
-  <si>
-    <t>Cápsulas Líquidas</t>
-  </si>
-  <si>
-    <t>Caja X 10</t>
-  </si>
-  <si>
-    <t>Pfizer</t>
-  </si>
-  <si>
-    <t>Liquido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calmidol Max </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 400Mg+65Mg Caja X 6</t>
-  </si>
-  <si>
-    <t>Tabletas Recubiertas</t>
-  </si>
-  <si>
-    <t>Sanofi</t>
+    <t>Atropina (clorhidrato)</t>
+  </si>
+  <si>
+    <t>1 mg/mL</t>
+  </si>
+  <si>
+    <t>pastillas</t>
+  </si>
+  <si>
+    <t>JGB</t>
+  </si>
+  <si>
+    <t>Blister x 10</t>
+  </si>
+  <si>
+    <t>Inyectable</t>
+  </si>
+  <si>
+    <t>cetirizina</t>
+  </si>
+  <si>
+    <t>10ml</t>
+  </si>
+  <si>
+    <t>GENFAR</t>
   </si>
   <si>
     <t>Tabletas</t>
   </si>
   <si>
-    <t xml:space="preserve">Creminem </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2% </t>
-  </si>
-  <si>
-    <t>Crema Vaginal Tubo x 20g</t>
-  </si>
-  <si>
-    <t>Mintlab</t>
-  </si>
-  <si>
-    <t>Crema</t>
-  </si>
-  <si>
-    <t>tópicas</t>
-  </si>
-  <si>
-    <t>Dolex Avanzado</t>
-  </si>
-  <si>
-    <t>500Mg Caja X 16</t>
-  </si>
-  <si>
-    <t>GLAXOSMITHKLINE COLOMBIA S.A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lumbal Caja </t>
-  </si>
-  <si>
-    <t>X 12 Tabletas</t>
-  </si>
-  <si>
-    <t>Contiene naproxeno y cafeína efectivo alivio del dolor de espalda</t>
-  </si>
-  <si>
-    <t>Nitrofurantoina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100Mg </t>
-  </si>
-  <si>
-    <t>Caja X 40 Cápsulas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oscillococcinum </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01Gr </t>
-  </si>
-  <si>
-    <t>x 6 Tabletas</t>
-  </si>
-  <si>
-    <t>Boiron</t>
-  </si>
-  <si>
-    <t>Gas medicinal</t>
-  </si>
-  <si>
-    <t>Inhalación</t>
-  </si>
-  <si>
-    <t>Pax Noche Granulos</t>
-  </si>
-  <si>
-    <t>Caja X 6</t>
-  </si>
-  <si>
-    <t>Sabor A Panela Limón</t>
-  </si>
-  <si>
-    <t>Sobre</t>
-  </si>
-  <si>
-    <t>Polvo</t>
-  </si>
-  <si>
-    <t>Sevedol Extra Fuerte</t>
-  </si>
-  <si>
-    <t>Caja X 8 Tabletas</t>
-  </si>
-  <si>
-    <t>Alivio contra el dolor fuerte de migraña</t>
+    <t>Glimepirida</t>
+  </si>
+  <si>
+    <t>4mg</t>
+  </si>
+  <si>
+    <t>Antidiabético oral</t>
+  </si>
+  <si>
+    <t>Mk</t>
+  </si>
+  <si>
+    <t>Metoclopramida</t>
+  </si>
+  <si>
+    <t>5mg/1mL</t>
+  </si>
+  <si>
+    <t>Es un antiemético</t>
+  </si>
+  <si>
+    <t>BAYER</t>
+  </si>
+  <si>
+    <t>Omeprazol</t>
+  </si>
+  <si>
+    <t>20mg</t>
+  </si>
+  <si>
+    <t>pastilla</t>
+  </si>
+  <si>
+    <t>Sucralfato</t>
+  </si>
+  <si>
+    <t>20g/100ml</t>
+  </si>
+  <si>
+    <t>Administración oral</t>
+  </si>
+  <si>
+    <t>Frasco</t>
   </si>
 </sst>
 </file>
@@ -557,20 +497,20 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A8" sqref="A8:I8"/>
+      <selection activeCell="A10" sqref="A10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="24" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="77" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="34" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="26" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="54" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="19" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="10" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -632,39 +572,37 @@
         <v>15</v>
       </c>
       <c r="H5">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="I5">
-        <v>7400</v>
+        <v>20500</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H6">
-        <v>139</v>
-      </c>
-      <c r="I6">
-        <v>16650</v>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3">
+        <v>1300</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -672,28 +610,28 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
         <v>15</v>
       </c>
       <c r="H7">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="I7">
-        <v>8700</v>
+        <v>56000</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -701,200 +639,80 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
-        <v>22500</v>
+        <v>6800</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H9">
-        <v>150</v>
-      </c>
-      <c r="I9">
-        <v>15950</v>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3">
+        <v>5500</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H10">
-        <v>149</v>
-      </c>
-      <c r="I10">
-        <v>18100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11">
-        <v>150</v>
-      </c>
-      <c r="I11">
-        <v>27700</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12">
-        <v>150</v>
-      </c>
-      <c r="I12">
-        <v>53900</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13">
-        <v>150</v>
-      </c>
-      <c r="I13">
-        <v>14750</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14">
-        <v>150</v>
-      </c>
-      <c r="I14">
-        <v>11800</v>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3">
+        <v>71000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de módulo gestión Lote parte 7,8,9 (Queda pendiente la generacion de pdf lote)
</commit_message>
<xml_diff>
--- a/Excel/reporte_productos.xlsx
+++ b/Excel/reporte_productos.xlsx
@@ -572,7 +572,7 @@
         <v>15</v>
       </c>
       <c r="H5">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="I5">
         <v>20500</v>
@@ -628,7 +628,7 @@
         <v>15</v>
       </c>
       <c r="H7">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>56000</v>

</xml_diff>

<commit_message>
Diseño final del sistema
</commit_message>
<xml_diff>
--- a/Excel/reporte_productos.xlsx
+++ b/Excel/reporte_productos.xlsx
@@ -687,31 +687,29 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H8">
-        <v>34</v>
-      </c>
-      <c r="I8">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3">
         <v>16000</v>
       </c>
     </row>
@@ -743,29 +741,31 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3">
+      <c r="H10">
+        <v>19</v>
+      </c>
+      <c r="I10">
         <v>56000</v>
       </c>
     </row>
@@ -872,27 +872,29 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="3">
+      <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
+      <c r="D15"/>
+      <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3">
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
         <v>5800</v>
       </c>
     </row>

</xml_diff>